<commit_message>
changeing uniform_id >> SubjectID
</commit_message>
<xml_diff>
--- a/Datasets/MECO/age_gender.xlsx
+++ b/Datasets/MECO/age_gender.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="613">
   <si>
-    <t>uniform_id</t>
+    <t>SubjectID</t>
   </si>
   <si>
     <t>Age</t>
@@ -1886,12 +1886,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1904,16 +1910,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1930,25 +1936,25 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1968,6 +1974,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -2167,17 +2174,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2205,10 +2212,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2456,12 +2463,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -2748,7 +2755,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2776,10 +2783,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>